<commit_message>
incorporating renv and output file
</commit_message>
<xml_diff>
--- a/data/GRB_veg-specs.xlsx
+++ b/data/GRB_veg-specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kim\Documents\Main Docs\Active Projects\Namaste\Namaste-Reserve-Final\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A467952-AEDB-40B3-BAE4-C9CE40C00B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFFBD51-99D9-4B9C-B0BC-3492692F0E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="624" yWindow="300" windowWidth="20316" windowHeight="11664" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ecotone_Migrators" sheetId="1" r:id="rId1"/>
@@ -1387,7 +1387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -31750,9 +31750,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>